<commit_message>
Changes on 15th January
</commit_message>
<xml_diff>
--- a/ProblemDefinition/XRayInput_new.xlsx
+++ b/ProblemDefinition/XRayInput_new.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Folder\Ali Documents\Job Documents\Hiwi\Hiwi - LPL - Eduardo\xray-matlab\v11\XRay\ProblemDefinition\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Folder\Ali Documents\Job Documents\Hiwi\Hiwi - LPL - Eduardo\xray-matlab\ProblemDefinition\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="25815" windowHeight="15495" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="25815" windowHeight="15495" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Design Variables" sheetId="1" r:id="rId1"/>
@@ -390,7 +390,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -414,7 +414,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -438,7 +438,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -462,7 +462,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -491,7 +491,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
   <si>
     <t>Variable Name</t>
   </si>
@@ -644,6 +644,12 @@
   </si>
   <si>
     <t>Design Var No</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>active</t>
   </si>
 </sst>
 </file>
@@ -1112,7 +1118,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -1183,10 +1189,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1195,12 +1201,13 @@
     <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="45.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" customWidth="1"/>
+    <col min="6" max="7" width="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1214,19 +1221,22 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -1237,15 +1247,18 @@
         <v>39</v>
       </c>
       <c r="E2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" t="s">
         <v>17</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>40</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>